<commit_message>
this is my update file of the project
</commit_message>
<xml_diff>
--- a/configurations/testdata.xlsx
+++ b/configurations/testdata.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="154">
   <si>
     <t>21914</t>
   </si>
@@ -445,6 +445,42 @@
   </si>
   <si>
     <t>75939</t>
+  </si>
+  <si>
+    <t>92156</t>
+  </si>
+  <si>
+    <t>77140</t>
+  </si>
+  <si>
+    <t>56442</t>
+  </si>
+  <si>
+    <t>69492</t>
+  </si>
+  <si>
+    <t>50443</t>
+  </si>
+  <si>
+    <t>23460</t>
+  </si>
+  <si>
+    <t>14171</t>
+  </si>
+  <si>
+    <t>81398</t>
+  </si>
+  <si>
+    <t>43346</t>
+  </si>
+  <si>
+    <t>69499</t>
+  </si>
+  <si>
+    <t>97410</t>
+  </si>
+  <si>
+    <t>1035</t>
   </si>
 </sst>
 </file>
@@ -771,7 +807,7 @@
   <sheetData>
     <row r="2">
       <c r="B2" t="s" s="0">
-        <v>141</v>
+        <v>153</v>
       </c>
     </row>
   </sheetData>

</xml_diff>